<commit_message>
Last commit before changing to Realistic Population
</commit_message>
<xml_diff>
--- a/WorkerCalc.xlsx
+++ b/WorkerCalc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Whitefang Greytail\Documents\Visual Studio 2019\Projects\WG_HouseholdCapacityModifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C68F73-86BA-4D0E-873E-58EFE157460C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48031007-832A-4C5B-8EFC-8945ADD241EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{837DFBAA-BE59-4B40-A14A-99C4D03947BD}"/>
   </bookViews>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3C188A-A917-4627-9F8C-CA03B9A0C4A5}">
-  <dimension ref="C1:H24"/>
+  <dimension ref="C1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,14 +461,14 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>0.5</v>
       </c>
       <c r="H4">
         <f>(C4*extra)*(D4*extra)*E4*F4*G4</f>
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
@@ -484,15 +484,15 @@
       </c>
       <c r="F5">
         <f>F4</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f>G4</f>
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f>(C5*extra)*(D5*extra)*E5*F5*G5</f>
-        <v>27</v>
+        <f t="shared" ref="H5:H12" si="0">(C5*extra)*(D5*extra)*E5*F5*G5</f>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
@@ -503,20 +503,20 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E12" si="0">E5</f>
+        <f t="shared" ref="E6:E12" si="1">E5</f>
         <v>3</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F12" si="1">F5</f>
-        <v>3</v>
+        <f t="shared" ref="F6:F12" si="2">F5</f>
+        <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G12" si="2">G5</f>
+        <f t="shared" ref="G6:G12" si="3">G5</f>
         <v>0.5</v>
       </c>
       <c r="H6">
-        <f>(C6*extra)*(D6*extra)*E6*F6*G6</f>
-        <v>40.5</v>
+        <f t="shared" si="0"/>
+        <v>13.5</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
@@ -527,20 +527,20 @@
         <v>5</v>
       </c>
       <c r="E7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="H7">
-        <f>(C7*extra)*(D7*extra)*E7*F7*G7</f>
-        <v>67.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -551,20 +551,20 @@
         <v>5</v>
       </c>
       <c r="E8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="H8">
-        <f>(C8*extra)*(D8*extra)*E8*F8*G8</f>
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
@@ -575,20 +575,20 @@
         <v>4</v>
       </c>
       <c r="E9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="H9">
-        <f>(C9*extra)*(D9*extra)*E9*F9*G9</f>
-        <v>72</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
@@ -599,20 +599,20 @@
         <v>5</v>
       </c>
       <c r="E10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="H10">
-        <f>(C10*extra)*(D10*extra)*E10*F10*G10</f>
-        <v>112.5</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
@@ -623,20 +623,20 @@
         <v>5</v>
       </c>
       <c r="E11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="H11">
-        <f>(C11*extra)*(D11*extra)*E11*F11*G11</f>
-        <v>135</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
@@ -647,20 +647,20 @@
         <v>6</v>
       </c>
       <c r="E12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="H12">
-        <f>(C12*extra)*(D12*extra)*E12*F12*G12</f>
-        <v>162</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
@@ -671,18 +671,18 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <f>5*MIN(C15,D15, 6)</f>
+        <f>5*MIN(FLOOR((C15+D15)/2, 1),6)</f>
         <v>10</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H15">
-        <f>(C15*extra)*(D15*extra)*E15*F15*G15</f>
-        <v>120</v>
+        <f t="shared" ref="H15:H23" si="4">(C15*extra)*(D15*extra)*E15*F15*G15</f>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
@@ -694,19 +694,19 @@
       </c>
       <c r="E16">
         <f>E15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F24" si="3">5*MIN(C16,D16, 6)</f>
+        <f t="shared" ref="F16:F26" si="5">5*MIN(FLOOR((C16+D16)/2, 1),6)</f>
         <v>10</v>
       </c>
       <c r="G16">
         <f>G15</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H16">
-        <f>(C16*extra)*(D16*extra)*E16*F16*G16</f>
-        <v>180</v>
+        <f t="shared" si="4"/>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
@@ -714,23 +714,23 @@
         <v>3</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E24" si="4">E16</f>
-        <v>3</v>
+        <f t="shared" ref="E17:E23" si="6">E16</f>
+        <v>4</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G24" si="5">G16</f>
-        <v>1</v>
+        <f t="shared" ref="G17:G24" si="7">G16</f>
+        <v>0.5</v>
       </c>
       <c r="H17">
-        <f>(C17*extra)*(D17*extra)*E17*F17*G17</f>
-        <v>405</v>
+        <f t="shared" si="4"/>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
@@ -741,20 +741,20 @@
         <v>5</v>
       </c>
       <c r="E18">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <f>(C18*extra)*(D18*extra)*E18*F18*G18</f>
-        <v>675</v>
+        <v>600</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
@@ -762,23 +762,23 @@
         <v>4</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <f>(C19*extra)*(D19*extra)*E19*F19*G19</f>
-        <v>1200</v>
+        <v>640</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
@@ -786,23 +786,23 @@
         <v>4</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <f>(C20*extra)*(D20*extra)*E20*F20*G20</f>
-        <v>960</v>
+        <v>800</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
@@ -813,20 +813,20 @@
         <v>5</v>
       </c>
       <c r="E21">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <f>(C21*extra)*(D21*extra)*E21*F21*G21</f>
-        <v>1875</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
@@ -837,20 +837,20 @@
         <v>5</v>
       </c>
       <c r="E22">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <f>(C22*extra)*(D22*extra)*E22*F22*G22</f>
-        <v>2250</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
@@ -861,44 +861,92 @@
         <v>6</v>
       </c>
       <c r="E23">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <f>(C23*extra)*(D23*extra)*E23*F23*G23</f>
-        <v>3240</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E24">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f>E22</f>
+        <v>4</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="G24">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24" si="8">(C24*extra)*(D24*extra)*E24*F24*G24</f>
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <f>E23</f>
+        <v>4</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <f>(C24*extra)*(D24*extra)*E24*F24*G24</f>
-        <v>25920</v>
+        <v>30</v>
+      </c>
+      <c r="G25">
+        <f>G24</f>
+        <v>0.5</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25" si="9">(C25*extra)*(D25*extra)*E25*F25*G25</f>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>14</v>
+      </c>
+      <c r="E26">
+        <f>E25</f>
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <f>G25</f>
+        <v>0.5</v>
+      </c>
+      <c r="H26">
+        <f>(C26*extra)*(D26*extra)*E26*F26*G26</f>
+        <v>10080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>